<commit_message>
Foram atualizadas as funções qtde_resultado_pag1() e rotina_buscar_endereco().
</commit_message>
<xml_diff>
--- a/Correios/A-Entrada/exemplo_1.xlsx
+++ b/Correios/A-Entrada/exemplo_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gst_9\Documents\bpa\Correios\A-Entrada\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gst_9\Documents\bpa\Correios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7DE11E-F89C-4520-8F58-50FC324AC75C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D77619-5006-4CC0-9A0D-07B0CE6312AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>agssgasgsagsagsaadg</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+  <si>
+    <t>CEP</t>
+  </si>
+  <si>
+    <t>96784-346</t>
+  </si>
+  <si>
+    <t>Rua Brinco de Princesa</t>
+  </si>
+  <si>
+    <t>a33</t>
+  </si>
+  <si>
+    <t>a##</t>
+  </si>
+  <si>
+    <t>sp</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>indigena</t>
   </si>
 </sst>
 </file>
@@ -71,9 +92,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D1" sqref="D1:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -367,13 +389,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>3840033</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>38400321</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="C3"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>38400322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>